<commit_message>
rate card import fix
</commit_message>
<xml_diff>
--- a/data/facilities_management/Direct Award Rate Cards - anonymised1.xlsx
+++ b/data/facilities_management/Direct Award Rate Cards - anonymised1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tariq/ccs/github/crown-marketplace/data/facilities_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F578D58A-B0B5-4247-B760-FAD31AC36FAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B58A20-29AB-FE47-B827-B12EFE1C38D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{E52F7FF7-80D8-A545-86A4-0E8FF36F8E0B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" activeTab="2" xr2:uid="{E52F7FF7-80D8-A545-86A4-0E8FF36F8E0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Prices" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9559" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9560" uniqueCount="152">
   <si>
     <t>Supplier</t>
   </si>
@@ -503,12 +503,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="12">
@@ -640,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -671,6 +677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1011,9 +1018,9 @@
   </sheetPr>
   <dimension ref="A1:Q1189"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -64078,7 +64085,7 @@
   <dimension ref="A1:D1189"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -80747,11 +80754,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBB1414-68A6-1D42-8FEC-665950336719}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -80767,7 +80774,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="11"/>
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="11" t="s">
         <v>118</v>
       </c>

</xml_diff>